<commit_message>
Current Cardmotron File for Bug report
</commit_message>
<xml_diff>
--- a/cards/BoardPandaGameCardmotron.xlsx
+++ b/cards/BoardPandaGameCardmotron.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\buerk\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\buerk\source\repos\the-board-game-idea\cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78BA62E-1FCC-4DD7-9D05-D3702FCE16CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66A5C4A-0A02-4F42-94DD-C9184D304F46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2301,8 +2301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2654,14 +2654,14 @@
         <v>380</v>
       </c>
       <c r="J21" s="17">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="K21" s="13"/>
       <c r="L21" s="7" t="s">
         <v>21</v>
       </c>
       <c r="M21" s="7">
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="N21" s="17" t="s">
         <v>49</v>
@@ -2693,7 +2693,7 @@
         <v>1200</v>
       </c>
       <c r="J22" s="17">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="K22" s="13"/>
       <c r="L22" s="7" t="s">
@@ -2734,14 +2734,14 @@
         <v>375</v>
       </c>
       <c r="J23" s="17">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K23" s="13"/>
       <c r="L23" s="7" t="s">
         <v>21</v>
       </c>
       <c r="M23" s="7">
-        <v>200</v>
+        <v>12</v>
       </c>
       <c r="N23" s="17" t="s">
         <v>47</v>
@@ -2773,14 +2773,14 @@
         <v>75</v>
       </c>
       <c r="J24" s="17">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="K24" s="13"/>
       <c r="L24" s="7" t="s">
         <v>21</v>
       </c>
       <c r="M24" s="7">
-        <v>200</v>
+        <v>75</v>
       </c>
       <c r="N24" s="17" t="s">
         <v>49</v>

</xml_diff>